<commit_message>
changing colors of correlations table
</commit_message>
<xml_diff>
--- a/sagol_project/04 - correlations/colored_results/comparing.xlsx
+++ b/sagol_project/04 - correlations/colored_results/comparing.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ליאור\Sagol_Reut_Naim_Project\sagol_project\04 - correlations\colored_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{857DFE6E-9DF2-4878-B9C2-091B2B550654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCFFBD5-7294-43DD-9B31-F9F5341D2A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DAC4EB0E-1DA6-483C-8E6F-EA714A6E14A9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="summary" sheetId="2" r:id="rId1"/>
+    <sheet name="origin" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">origin!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">summary!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
   <si>
     <t>ARI_6_P</t>
   </si>
@@ -222,13 +227,25 @@
   </si>
   <si>
     <t>pctOffscreen.a_a</t>
+  </si>
+  <si>
+    <t>ARI_6_P2</t>
+  </si>
+  <si>
+    <t>SCARED_P3</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Greater anxiety is associated with increased fixations on the mouth and reduced attention to the eyes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,8 +278,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="20">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,8 +408,134 @@
         <bgColor rgb="FF16AAAA"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF02AAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF16AAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF04AAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF11AAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF05AAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF03AAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF09AAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF07AAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF0BAAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF0DAAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF12AAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF01AAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FF09AAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF0CAAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF0DAAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF0AAAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF01AAAA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF10AAAA"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -386,11 +543,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -416,11 +684,209 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="38" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="40" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -431,6 +897,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47603EAD-4F07-485D-8BDD-D8213AF775EB}" name="Table1" displayName="Table1" ref="A1:F18" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:F18" xr:uid="{47603EAD-4F07-485D-8BDD-D8213AF775EB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F18">
+    <sortCondition ref="D1:D18"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{51DD47E8-2062-4E37-80B5-2F6DD310787A}" name="Feature" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{AD5E388C-8732-487F-8693-8ECF55F1D948}" name="ARI_6_P" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{CE844878-A641-4AE8-8FB6-312C18F5F50B}" name="SCARED_P" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{986E0538-7ED1-4A19-B43E-51425A764529}" name="ARI_6_P2" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{C5A2EE4F-93A0-4DCF-B389-D40930423B05}" name="SCARED_P3" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{7E8B04CB-2D85-4EA9-A9E7-7F3D0273C106}" name="notes" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -749,11 +1233,367 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B578667A-2680-49D3-B6F8-07D5B250D589}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.58203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.58203125" customWidth="1"/>
+    <col min="6" max="6" width="82.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="23">
+        <v>1</v>
+      </c>
+      <c r="C2" s="23">
+        <v>0.4474535361402916</v>
+      </c>
+      <c r="D2" s="23">
+        <v>0</v>
+      </c>
+      <c r="E2" s="24">
+        <v>1.4268712578451E-3</v>
+      </c>
+      <c r="F2" s="25"/>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23">
+        <v>0.44745353614029171</v>
+      </c>
+      <c r="C3" s="23">
+        <v>1</v>
+      </c>
+      <c r="D3" s="24">
+        <v>1.4268712578451E-3</v>
+      </c>
+      <c r="E3" s="23">
+        <v>0</v>
+      </c>
+      <c r="F3" s="25"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="28">
+        <v>0.38472310633835538</v>
+      </c>
+      <c r="C4" s="28">
+        <v>0.28405431137307019</v>
+      </c>
+      <c r="D4" s="47">
+        <v>1.0290865557569501E-2</v>
+      </c>
+      <c r="E4" s="64">
+        <v>8.70135228415687E-2</v>
+      </c>
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="28">
+        <v>0.362600398731179</v>
+      </c>
+      <c r="C5" s="28">
+        <v>0.29813747807272051</v>
+      </c>
+      <c r="D5" s="48">
+        <v>1.7737420230970299E-2</v>
+      </c>
+      <c r="E5" s="63">
+        <v>6.7169170722953697E-2</v>
+      </c>
+      <c r="F5" s="25"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="28">
+        <v>-0.3522960440065947</v>
+      </c>
+      <c r="C6" s="28">
+        <v>-0.37700393844585628</v>
+      </c>
+      <c r="D6" s="49">
+        <v>2.21877356247113E-2</v>
+      </c>
+      <c r="E6" s="57">
+        <v>1.2448974568196301E-2</v>
+      </c>
+      <c r="F6" s="25"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="29">
+        <v>0.33013541275526698</v>
+      </c>
+      <c r="C7" s="29">
+        <v>0.24438648708217151</v>
+      </c>
+      <c r="D7" s="50">
+        <v>3.6065399172333999E-2</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0.16678582915720319</v>
+      </c>
+      <c r="F7" s="25"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="28">
+        <v>0.32747921348827608</v>
+      </c>
+      <c r="C8" s="28">
+        <v>0.3370484429092751</v>
+      </c>
+      <c r="D8" s="51">
+        <v>3.7863208924659199E-2</v>
+      </c>
+      <c r="E8" s="58">
+        <v>3.1021653113081901E-2</v>
+      </c>
+      <c r="F8" s="25"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="28">
+        <v>0.3208830621259981</v>
+      </c>
+      <c r="C9" s="28">
+        <v>0.35778599547286649</v>
+      </c>
+      <c r="D9" s="52">
+        <v>4.3310046009072803E-2</v>
+      </c>
+      <c r="E9" s="49">
+        <v>1.9779123534089602E-2</v>
+      </c>
+      <c r="F9" s="25"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="28">
+        <v>0.31257575297444329</v>
+      </c>
+      <c r="C10" s="28">
+        <v>0.35894740071726489</v>
+      </c>
+      <c r="D10" s="53">
+        <v>5.1059801522941699E-2</v>
+      </c>
+      <c r="E10" s="48">
+        <v>1.93090988303498E-2</v>
+      </c>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="28">
+        <v>-0.29306352033085908</v>
+      </c>
+      <c r="C11" s="28">
+        <v>-0.40033414379574189</v>
+      </c>
+      <c r="D11" s="54">
+        <v>7.3669968135166103E-2</v>
+      </c>
+      <c r="E11" s="55">
+        <v>6.9151548725863996E-3</v>
+      </c>
+      <c r="F11" s="25"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="30">
+        <v>0.26982593286162881</v>
+      </c>
+      <c r="C12" s="30">
+        <v>0.31491656386503608</v>
+      </c>
+      <c r="D12" s="30">
+        <v>0.1123547409265663</v>
+      </c>
+      <c r="E12" s="60">
+        <v>4.8955247764224101E-2</v>
+      </c>
+      <c r="F12" s="32"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="23">
+        <v>-0.26237535719668309</v>
+      </c>
+      <c r="C13" s="23">
+        <v>-0.39812795820732633</v>
+      </c>
+      <c r="D13" s="23">
+        <v>0.12640111374424051</v>
+      </c>
+      <c r="E13" s="56">
+        <v>7.2956532922877999E-3</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="30">
+        <v>-0.24455018157045369</v>
+      </c>
+      <c r="C14" s="30">
+        <v>-0.30997755993737669</v>
+      </c>
+      <c r="D14" s="30">
+        <v>0.1667755620293975</v>
+      </c>
+      <c r="E14" s="61">
+        <v>5.3723290982506902E-2</v>
+      </c>
+      <c r="F14" s="32"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="30">
+        <v>-0.2250771642525087</v>
+      </c>
+      <c r="C15" s="30">
+        <v>-0.32501820120360569</v>
+      </c>
+      <c r="D15" s="30">
+        <v>0.21353043464389801</v>
+      </c>
+      <c r="E15" s="59">
+        <v>3.9700775402616198E-2</v>
+      </c>
+      <c r="F15" s="32"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="31">
+        <v>-0.20942554051778159</v>
+      </c>
+      <c r="C16" s="31">
+        <v>-0.39551611728149211</v>
+      </c>
+      <c r="D16" s="31">
+        <v>0.25784975272580968</v>
+      </c>
+      <c r="E16" s="65">
+        <v>7.8186434898968992E-3</v>
+      </c>
+      <c r="F16" s="33"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="30">
+        <v>-6.9241075036134803E-2</v>
+      </c>
+      <c r="C17" s="30">
+        <v>-0.29382936376435198</v>
+      </c>
+      <c r="D17" s="30">
+        <v>0.762588368906856</v>
+      </c>
+      <c r="E17" s="62">
+        <v>6.6543060469132095E-2</v>
+      </c>
+      <c r="F17" s="27"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="45">
+        <v>5.48044590724081E-2</v>
+      </c>
+      <c r="C18" s="45">
+        <v>0.25638425818193089</v>
+      </c>
+      <c r="D18" s="45">
+        <v>0.81507762335136802</v>
+      </c>
+      <c r="E18" s="45">
+        <v>0.1391351994731275</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B20D8A-57A7-48F7-BFD3-87485132E59A}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1799,6 +2639,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{A1B20D8A-57A7-48F7-BFD3-87485132E59A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>